<commit_message>
add appropriate validations, configurations for contact types and icons and forms
</commit_message>
<xml_diff>
--- a/POSHIT/Example CHT application/malaria-usecase-cht/forms/app/children_under_5_follow_up.xlsx
+++ b/POSHIT/Example CHT application/malaria-usecase-cht/forms/app/children_under_5_follow_up.xlsx
@@ -446,6 +446,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">worsening</t>
     </r>
@@ -480,6 +481,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">cured</t>
     </r>
@@ -597,6 +599,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1122,11 +1125,11 @@
   </sheetPr>
   <dimension ref="A1:AJ67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C58" activeCellId="0" sqref="C58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="40:40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.55"/>
@@ -3829,10 +3832,10 @@
   <dimension ref="A1:V1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="1" sqref="40:40 B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="2" style="35" width="45.84"/>
@@ -4070,10 +4073,10 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="40:40 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.83"/>
@@ -4130,7 +4133,7 @@
       </c>
       <c r="C2" s="49" t="n">
         <f aca="true">NOW()</f>
-        <v>45090.6747921472</v>
+        <v>45096.5331461243</v>
       </c>
       <c r="D2" s="50" t="s">
         <v>167</v>

</xml_diff>

<commit_message>
update codebase with forms , icons and targets
</commit_message>
<xml_diff>
--- a/POSHIT/Example CHT application/malaria-usecase-cht/forms/app/children_under_5_follow_up.xlsx
+++ b/POSHIT/Example CHT application/malaria-usecase-cht/forms/app/children_under_5_follow_up.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="174">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -270,10 +270,16 @@
     <t xml:space="preserve">../inputs/contact/name</t>
   </si>
   <si>
+    <t xml:space="preserve">calculated_follow_up_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if(../follow_up_details/follow_up_date != ‘', ../follow_up_details/follow_up_date, date-time(decimal-date-time(today()) + 3))</t>
+  </si>
+  <si>
     <t xml:space="preserve">referral_follow_up_date</t>
   </si>
   <si>
-    <t xml:space="preserve">date-time(decimal-date-time(today()) + 3)</t>
+    <t xml:space="preserve">if(../children_under_5_follow_up/no_follow_up_required = 'true',  '', ${calculated_follow_up_date} ) </t>
   </si>
   <si>
     <t xml:space="preserve">follow_up_details</t>
@@ -355,6 +361,12 @@
   </si>
   <si>
     <t xml:space="preserve">Have you referred ${patient_name} to the health facility?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no_follow_up_required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(${child_condition}, ‘improving’) or selected(${child_condition}, ‘cured’) </t>
   </si>
   <si>
     <t xml:space="preserve">group_review</t>
@@ -1123,13 +1135,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AJ67"/>
+  <dimension ref="A1:AJ69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="40:40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L35" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P41" activeCellId="0" sqref="P41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.55"/>
@@ -1141,7 +1153,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="28.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="35.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="39.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="132.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="23.99"/>
   </cols>
   <sheetData>
@@ -2887,10 +2899,10 @@
       <c r="AJ39" s="16"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="18" t="s">
+      <c r="A40" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="13" t="s">
         <v>82</v>
       </c>
       <c r="C40" s="14" t="s">
@@ -2902,139 +2914,144 @@
       <c r="G40" s="15"/>
       <c r="H40" s="15"/>
       <c r="I40" s="15"/>
-      <c r="J40" s="15"/>
-      <c r="K40" s="15"/>
-      <c r="L40" s="15"/>
-      <c r="M40" s="15"/>
-      <c r="N40" s="15"/>
-      <c r="O40" s="15"/>
-      <c r="P40" s="16" t="s">
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="16"/>
+      <c r="N40" s="16"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="Q40" s="15"/>
-      <c r="R40" s="15"/>
-      <c r="S40" s="15"/>
-      <c r="T40" s="15"/>
-      <c r="V40" s="15"/>
-      <c r="W40" s="15"/>
-      <c r="X40" s="15"/>
-      <c r="Y40" s="15"/>
-      <c r="Z40" s="15"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="14"/>
+      <c r="S40" s="14"/>
+      <c r="T40" s="14"/>
+      <c r="V40" s="16"/>
+      <c r="W40" s="16"/>
+      <c r="X40" s="16"/>
+      <c r="Y40" s="16"/>
+      <c r="Z40" s="16"/>
       <c r="AA40" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="AB40" s="15"/>
-      <c r="AC40" s="15"/>
-      <c r="AD40" s="15"/>
-      <c r="AE40" s="15"/>
-      <c r="AG40" s="15"/>
+      <c r="AB40" s="16"/>
+      <c r="AC40" s="16"/>
+      <c r="AD40" s="16"/>
+      <c r="AE40" s="16"/>
+      <c r="AG40" s="16"/>
       <c r="AH40" s="16"/>
       <c r="AI40" s="16"/>
       <c r="AJ40" s="16"/>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B42" s="0" t="s">
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="G42" s="0" t="s">
-        <v>33</v>
-      </c>
+      <c r="C41" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="15"/>
+      <c r="O41" s="15"/>
+      <c r="P41" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q41" s="15"/>
+      <c r="R41" s="15"/>
+      <c r="S41" s="15"/>
+      <c r="T41" s="15"/>
+      <c r="V41" s="15"/>
+      <c r="W41" s="15"/>
+      <c r="X41" s="15"/>
+      <c r="Y41" s="15"/>
+      <c r="Z41" s="15"/>
+      <c r="AA41" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB41" s="15"/>
+      <c r="AC41" s="15"/>
+      <c r="AD41" s="15"/>
+      <c r="AE41" s="15"/>
+      <c r="AG41" s="15"/>
+      <c r="AH41" s="16"/>
+      <c r="AI41" s="16"/>
+      <c r="AJ41" s="16"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="C43" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>88</v>
+      <c r="G43" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="E44" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="F44" s="0" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B47" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="G47" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
-      <c r="J47" s="20"/>
-      <c r="K47" s="20"/>
-      <c r="L47" s="20"/>
-      <c r="M47" s="20"/>
-      <c r="N47" s="20"/>
-      <c r="O47" s="20"/>
-      <c r="P47" s="20"/>
-      <c r="Q47" s="20"/>
-      <c r="R47" s="20"/>
-      <c r="S47" s="20"/>
-      <c r="T47" s="20"/>
-      <c r="U47" s="20"/>
-      <c r="V47" s="20"/>
-      <c r="W47" s="20"/>
-      <c r="X47" s="20"/>
-      <c r="Y47" s="20"/>
-      <c r="Z47" s="20"/>
-      <c r="AA47" s="20"/>
-      <c r="AB47" s="20"/>
-      <c r="AC47" s="20"/>
-      <c r="AD47" s="20"/>
-      <c r="AE47" s="20"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="B48" s="19" t="s">
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="C48" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F48" s="20"/>
-      <c r="G48" s="20"/>
+      <c r="G48" s="20" t="s">
+        <v>33</v>
+      </c>
       <c r="H48" s="20"/>
       <c r="I48" s="20"/>
       <c r="J48" s="20"/>
@@ -3062,19 +3079,19 @@
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="19" t="s">
+      <c r="C49" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="C49" s="20" t="s">
-        <v>101</v>
-      </c>
       <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20" t="s">
-        <v>102</v>
-      </c>
+      <c r="E49" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F49" s="20"/>
       <c r="G49" s="20"/>
       <c r="H49" s="20"/>
       <c r="I49" s="20"/>
@@ -3103,18 +3120,18 @@
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="19" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B50" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C50" s="20" t="s">
         <v>103</v>
-      </c>
-      <c r="C50" s="20" t="s">
-        <v>104</v>
       </c>
       <c r="D50" s="20"/>
       <c r="E50" s="20"/>
       <c r="F50" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G50" s="20"/>
       <c r="H50" s="20"/>
@@ -3144,18 +3161,18 @@
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="19" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B51" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" s="20" t="s">
         <v>106</v>
-      </c>
-      <c r="C51" s="20" t="s">
-        <v>107</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="20"/>
       <c r="F51" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G51" s="20"/>
       <c r="H51" s="20"/>
@@ -3185,20 +3202,18 @@
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="19" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="B52" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C52" s="20" t="s">
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20" t="s">
         <v>110</v>
-      </c>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F52" s="20" t="s">
-        <v>108</v>
       </c>
       <c r="G52" s="20"/>
       <c r="H52" s="20"/>
@@ -3228,13 +3243,21 @@
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B53" s="19"/>
-      <c r="C53" s="20"/>
+        <v>87</v>
+      </c>
+      <c r="B53" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>112</v>
+      </c>
       <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
+      <c r="E53" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F53" s="20" t="s">
+        <v>110</v>
+      </c>
       <c r="G53" s="20"/>
       <c r="H53" s="20"/>
       <c r="I53" s="20"/>
@@ -3261,145 +3284,116 @@
       <c r="AD53" s="20"/>
       <c r="AE53" s="20"/>
     </row>
-    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="21" t="s">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P54" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B55" s="19"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="20"/>
+      <c r="I55" s="20"/>
+      <c r="J55" s="20"/>
+      <c r="K55" s="20"/>
+      <c r="L55" s="20"/>
+      <c r="M55" s="20"/>
+      <c r="N55" s="20"/>
+      <c r="O55" s="20"/>
+      <c r="P55" s="20"/>
+      <c r="Q55" s="20"/>
+      <c r="R55" s="20"/>
+      <c r="S55" s="20"/>
+      <c r="T55" s="20"/>
+      <c r="U55" s="20"/>
+      <c r="V55" s="20"/>
+      <c r="W55" s="20"/>
+      <c r="X55" s="20"/>
+      <c r="Y55" s="20"/>
+      <c r="Z55" s="20"/>
+      <c r="AA55" s="20"/>
+      <c r="AB55" s="20"/>
+      <c r="AC55" s="20"/>
+      <c r="AD55" s="20"/>
+      <c r="AE55" s="20"/>
+    </row>
+    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B54" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="C54" s="23" t="s">
+      <c r="B56" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C56" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="D54" s="24" t="s">
+      <c r="D56" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E54" s="25"/>
-      <c r="F54" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="G54" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="H54" s="26"/>
-      <c r="I54" s="26"/>
-      <c r="J54" s="26"/>
-      <c r="K54" s="27"/>
-      <c r="L54" s="26"/>
-      <c r="M54" s="28" t="s">
+      <c r="E56" s="25"/>
+      <c r="F56" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="G56" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="H56" s="26"/>
+      <c r="I56" s="26"/>
+      <c r="J56" s="26"/>
+      <c r="K56" s="27"/>
+      <c r="L56" s="26"/>
+      <c r="M56" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="N54" s="26"/>
-      <c r="O54" s="26"/>
-      <c r="P54" s="29"/>
-      <c r="Q54" s="29"/>
-      <c r="R54" s="29"/>
-      <c r="S54" s="29"/>
-      <c r="T54" s="29"/>
-      <c r="U54" s="29"/>
-      <c r="V54" s="29"/>
-      <c r="W54" s="29"/>
-      <c r="X54" s="29"/>
-      <c r="Y54" s="29"/>
-      <c r="Z54" s="29"/>
-      <c r="AA54" s="30"/>
-      <c r="AB54" s="30"/>
-    </row>
-    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="B55" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="C55" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="D55" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="E55" s="31"/>
-      <c r="F55" s="32"/>
-      <c r="G55" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="H55" s="32"/>
-      <c r="I55" s="32"/>
-      <c r="J55" s="32"/>
-      <c r="K55" s="27"/>
-      <c r="L55" s="32"/>
-      <c r="M55" s="32"/>
-      <c r="N55" s="32"/>
-      <c r="O55" s="32"/>
-      <c r="P55" s="32"/>
-      <c r="Q55" s="32"/>
-      <c r="R55" s="32"/>
-      <c r="S55" s="32"/>
-      <c r="T55" s="32"/>
-      <c r="U55" s="32"/>
-      <c r="V55" s="32"/>
-      <c r="W55" s="32"/>
-      <c r="X55" s="32"/>
-      <c r="Y55" s="32"/>
-      <c r="Z55" s="32"/>
-      <c r="AA55" s="30"/>
-      <c r="AB55" s="30"/>
-    </row>
-    <row r="56" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="B56" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="C56" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="D56" s="24"/>
-      <c r="E56" s="33"/>
-      <c r="F56" s="34"/>
-      <c r="G56" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="H56" s="32"/>
-      <c r="I56" s="32"/>
-      <c r="J56" s="32"/>
-      <c r="K56" s="27"/>
-      <c r="L56" s="32"/>
-      <c r="M56" s="32"/>
-      <c r="N56" s="32"/>
-      <c r="O56" s="32"/>
-      <c r="P56" s="32"/>
-      <c r="Q56" s="32"/>
-      <c r="R56" s="32"/>
-      <c r="S56" s="32"/>
-      <c r="T56" s="32"/>
-      <c r="U56" s="32"/>
-      <c r="V56" s="32"/>
-      <c r="W56" s="32"/>
-      <c r="X56" s="32"/>
-      <c r="Y56" s="32"/>
-      <c r="Z56" s="32"/>
+      <c r="N56" s="26"/>
+      <c r="O56" s="26"/>
+      <c r="P56" s="29"/>
+      <c r="Q56" s="29"/>
+      <c r="R56" s="29"/>
+      <c r="S56" s="29"/>
+      <c r="T56" s="29"/>
+      <c r="U56" s="29"/>
+      <c r="V56" s="29"/>
+      <c r="W56" s="29"/>
+      <c r="X56" s="29"/>
+      <c r="Y56" s="29"/>
+      <c r="Z56" s="29"/>
       <c r="AA56" s="30"/>
       <c r="AB56" s="30"/>
     </row>
-    <row r="57" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="B57" s="33" t="s">
+    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B57" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="C57" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="D57" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="E57" s="31"/>
+      <c r="F57" s="32"/>
+      <c r="G57" s="31" t="s">
         <v>120</v>
-      </c>
-      <c r="C57" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="D57" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="E57" s="33"/>
-      <c r="F57" s="34"/>
-      <c r="G57" s="33" t="s">
-        <v>123</v>
       </c>
       <c r="H57" s="32"/>
       <c r="I57" s="32"/>
@@ -3425,19 +3419,19 @@
     </row>
     <row r="58" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="33" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B58" s="33" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C58" s="23" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D58" s="24"/>
       <c r="E58" s="33"/>
       <c r="F58" s="34"/>
       <c r="G58" s="22" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="H58" s="32"/>
       <c r="I58" s="32"/>
@@ -3463,19 +3457,21 @@
     </row>
     <row r="59" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="33" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B59" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="C59" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="D59" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="C59" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="D59" s="24"/>
       <c r="E59" s="33"/>
       <c r="F59" s="34"/>
-      <c r="G59" s="22" t="s">
-        <v>119</v>
+      <c r="G59" s="33" t="s">
+        <v>127</v>
       </c>
       <c r="H59" s="32"/>
       <c r="I59" s="32"/>
@@ -3501,19 +3497,19 @@
     </row>
     <row r="60" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="B60" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B60" s="33" t="s">
         <v>128</v>
       </c>
       <c r="C60" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="D60" s="22"/>
-      <c r="E60" s="22"/>
-      <c r="F60" s="25"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="33"/>
+      <c r="F60" s="34"/>
       <c r="G60" s="22" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="H60" s="32"/>
       <c r="I60" s="32"/>
@@ -3539,21 +3535,19 @@
     </row>
     <row r="61" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="B61" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B61" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="C61" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="C61" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="D61" s="22"/>
-      <c r="E61" s="22"/>
-      <c r="F61" s="25" t="s">
-        <v>133</v>
-      </c>
+      <c r="D61" s="24"/>
+      <c r="E61" s="33"/>
+      <c r="F61" s="34"/>
       <c r="G61" s="22" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="H61" s="32"/>
       <c r="I61" s="32"/>
@@ -3579,21 +3573,19 @@
     </row>
     <row r="62" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="33" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C62" s="23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D62" s="22"/>
       <c r="E62" s="22"/>
-      <c r="F62" s="25" t="s">
-        <v>136</v>
-      </c>
+      <c r="F62" s="25"/>
       <c r="G62" s="22" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="H62" s="32"/>
       <c r="I62" s="32"/>
@@ -3619,21 +3611,21 @@
     </row>
     <row r="63" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="33" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C63" s="23" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D63" s="22"/>
       <c r="E63" s="22"/>
       <c r="F63" s="25" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G63" s="22" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="H63" s="32"/>
       <c r="I63" s="32"/>
@@ -3659,21 +3651,21 @@
     </row>
     <row r="64" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="33" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C64" s="23" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D64" s="22"/>
       <c r="E64" s="22"/>
       <c r="F64" s="25" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="G64" s="22" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="H64" s="32"/>
       <c r="I64" s="32"/>
@@ -3699,19 +3691,21 @@
     </row>
     <row r="65" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="33" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B65" s="22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C65" s="23" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D65" s="22"/>
       <c r="E65" s="22"/>
-      <c r="F65" s="25"/>
+      <c r="F65" s="25" t="s">
+        <v>143</v>
+      </c>
       <c r="G65" s="22" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="H65" s="32"/>
       <c r="I65" s="32"/>
@@ -3737,19 +3731,21 @@
     </row>
     <row r="66" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="33" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B66" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="C66" s="23" t="s">
         <v>145</v>
-      </c>
-      <c r="C66" s="23" t="s">
-        <v>146</v>
       </c>
       <c r="D66" s="22"/>
       <c r="E66" s="22"/>
-      <c r="F66" s="25"/>
+      <c r="F66" s="25" t="s">
+        <v>140</v>
+      </c>
       <c r="G66" s="22" t="s">
-        <v>119</v>
+        <v>146</v>
       </c>
       <c r="H66" s="32"/>
       <c r="I66" s="32"/>
@@ -3773,43 +3769,119 @@
       <c r="AA66" s="30"/>
       <c r="AB66" s="30"/>
     </row>
-    <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="H67" s="29"/>
-      <c r="I67" s="29"/>
+    <row r="67" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B67" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="C67" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="D67" s="22"/>
+      <c r="E67" s="22"/>
+      <c r="F67" s="25"/>
+      <c r="G67" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="H67" s="32"/>
+      <c r="I67" s="32"/>
       <c r="J67" s="32"/>
       <c r="K67" s="27"/>
-      <c r="L67" s="29"/>
-      <c r="M67" s="29"/>
-      <c r="N67" s="29"/>
-      <c r="O67" s="29"/>
-      <c r="P67" s="29"/>
-      <c r="Q67" s="29"/>
-      <c r="R67" s="29"/>
-      <c r="S67" s="29"/>
-      <c r="T67" s="29"/>
-      <c r="U67" s="29"/>
-      <c r="V67" s="29"/>
-      <c r="W67" s="29"/>
-      <c r="X67" s="29"/>
-      <c r="Y67" s="29"/>
-      <c r="Z67" s="29"/>
+      <c r="L67" s="32"/>
+      <c r="M67" s="32"/>
+      <c r="N67" s="32"/>
+      <c r="O67" s="32"/>
+      <c r="P67" s="32"/>
+      <c r="Q67" s="32"/>
+      <c r="R67" s="32"/>
+      <c r="S67" s="32"/>
+      <c r="T67" s="32"/>
+      <c r="U67" s="32"/>
+      <c r="V67" s="32"/>
+      <c r="W67" s="32"/>
+      <c r="X67" s="32"/>
+      <c r="Y67" s="32"/>
+      <c r="Z67" s="32"/>
       <c r="AA67" s="30"/>
       <c r="AB67" s="30"/>
     </row>
+    <row r="68" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B68" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="C68" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="D68" s="22"/>
+      <c r="E68" s="22"/>
+      <c r="F68" s="25"/>
+      <c r="G68" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="H68" s="32"/>
+      <c r="I68" s="32"/>
+      <c r="J68" s="32"/>
+      <c r="K68" s="27"/>
+      <c r="L68" s="32"/>
+      <c r="M68" s="32"/>
+      <c r="N68" s="32"/>
+      <c r="O68" s="32"/>
+      <c r="P68" s="32"/>
+      <c r="Q68" s="32"/>
+      <c r="R68" s="32"/>
+      <c r="S68" s="32"/>
+      <c r="T68" s="32"/>
+      <c r="U68" s="32"/>
+      <c r="V68" s="32"/>
+      <c r="W68" s="32"/>
+      <c r="X68" s="32"/>
+      <c r="Y68" s="32"/>
+      <c r="Z68" s="32"/>
+      <c r="AA68" s="30"/>
+      <c r="AB68" s="30"/>
+    </row>
+    <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="H69" s="29"/>
+      <c r="I69" s="29"/>
+      <c r="J69" s="32"/>
+      <c r="K69" s="27"/>
+      <c r="L69" s="29"/>
+      <c r="M69" s="29"/>
+      <c r="N69" s="29"/>
+      <c r="O69" s="29"/>
+      <c r="P69" s="29"/>
+      <c r="Q69" s="29"/>
+      <c r="R69" s="29"/>
+      <c r="S69" s="29"/>
+      <c r="T69" s="29"/>
+      <c r="U69" s="29"/>
+      <c r="V69" s="29"/>
+      <c r="W69" s="29"/>
+      <c r="X69" s="29"/>
+      <c r="Y69" s="29"/>
+      <c r="Z69" s="29"/>
+      <c r="AA69" s="30"/>
+      <c r="AB69" s="30"/>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E47:E53" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E48:E53 E55" type="list">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="A2:A40" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="A2:A41" type="list">
       <formula1>"note,select_one,select_multiple,date,time,calculate,integer,text,decimal,acknowledge,dateTime,image,range,begin group,end group,hidden,db:person,db:clinic,db:health_center,db:district_hospital,string"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="J2:J40" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="J2:J41" type="list">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3832,10 +3904,10 @@
   <dimension ref="A1:V1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="1" sqref="40:40 B8"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.59765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="2" style="35" width="45.84"/>
@@ -3843,7 +3915,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="36" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B1" s="36" t="s">
         <v>1</v>
@@ -3852,22 +3924,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="38" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="E1" s="39" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="F1" s="40" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="H1" s="42" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="I1" s="43" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="J1" s="44"/>
       <c r="K1" s="44"/>
@@ -3885,13 +3957,13 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="44" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B2" s="44" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C2" s="45" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D2" s="46"/>
       <c r="E2" s="46"/>
@@ -3915,13 +3987,13 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="44" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C3" s="45" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="D3" s="46"/>
       <c r="E3" s="46"/>
@@ -3969,35 +4041,35 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="35" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="35" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="35" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4073,10 +4145,10 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="40:40 A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.83"/>
@@ -4084,25 +4156,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="36" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E1" s="36" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="G1" s="47" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="H1" s="36"/>
       <c r="I1" s="36"/>
@@ -4126,24 +4198,24 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="48" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C2" s="49" t="n">
         <f aca="true">NOW()</f>
-        <v>45096.5331461243</v>
+        <v>45113.8452357324</v>
       </c>
       <c r="D2" s="50" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F2" s="44"/>
       <c r="G2" s="51" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H2" s="44"/>
       <c r="I2" s="44"/>

</xml_diff>

<commit_message>
updated form configuration and settings and added targets and summaries
</commit_message>
<xml_diff>
--- a/POSHIT/Example CHT application/malaria-usecase-cht/forms/app/children_under_5_follow_up.xlsx
+++ b/POSHIT/Example CHT application/malaria-usecase-cht/forms/app/children_under_5_follow_up.xlsx
@@ -1135,13 +1135,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AJ69"/>
+  <dimension ref="A1:AJ68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L35" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P41" activeCellId="0" sqref="P41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.55"/>
@@ -2990,68 +2990,109 @@
       <c r="AI41" s="16"/>
       <c r="AJ41" s="16"/>
     </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="G43" s="0" t="s">
-        <v>33</v>
+        <v>88</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
         <v>48</v>
       </c>
+    </row>
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="G47" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="H47" s="20"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="20"/>
+      <c r="K47" s="20"/>
+      <c r="L47" s="20"/>
+      <c r="M47" s="20"/>
+      <c r="N47" s="20"/>
+      <c r="O47" s="20"/>
+      <c r="P47" s="20"/>
+      <c r="Q47" s="20"/>
+      <c r="R47" s="20"/>
+      <c r="S47" s="20"/>
+      <c r="T47" s="20"/>
+      <c r="U47" s="20"/>
+      <c r="V47" s="20"/>
+      <c r="W47" s="20"/>
+      <c r="X47" s="20"/>
+      <c r="Y47" s="20"/>
+      <c r="Z47" s="20"/>
+      <c r="AA47" s="20"/>
+      <c r="AB47" s="20"/>
+      <c r="AC47" s="20"/>
+      <c r="AD47" s="20"/>
+      <c r="AE47" s="20"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="19" t="s">
-        <v>29</v>
+        <v>98</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="G48" s="20" t="s">
-        <v>33</v>
-      </c>
+      <c r="E48" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
       <c r="H48" s="20"/>
       <c r="I48" s="20"/>
       <c r="J48" s="20"/>
@@ -3079,19 +3120,19 @@
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="19" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D49" s="20"/>
-      <c r="E49" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="F49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20" t="s">
+        <v>104</v>
+      </c>
       <c r="G49" s="20"/>
       <c r="H49" s="20"/>
       <c r="I49" s="20"/>
@@ -3123,15 +3164,15 @@
         <v>101</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D50" s="20"/>
       <c r="E50" s="20"/>
       <c r="F50" s="20" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="G50" s="20"/>
       <c r="H50" s="20"/>
@@ -3164,15 +3205,15 @@
         <v>101</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="20"/>
       <c r="F51" s="20" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="G51" s="20"/>
       <c r="H51" s="20"/>
@@ -3202,16 +3243,18 @@
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="19" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C52" s="20" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
+      <c r="E52" s="20" t="s">
+        <v>90</v>
+      </c>
       <c r="F52" s="20" t="s">
         <v>110</v>
       </c>
@@ -3241,159 +3284,154 @@
       <c r="AD52" s="20"/>
       <c r="AE52" s="20"/>
     </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="B53" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="C53" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="F53" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="G53" s="20"/>
-      <c r="H53" s="20"/>
-      <c r="I53" s="20"/>
-      <c r="J53" s="20"/>
-      <c r="K53" s="20"/>
-      <c r="L53" s="20"/>
-      <c r="M53" s="20"/>
-      <c r="N53" s="20"/>
-      <c r="O53" s="20"/>
-      <c r="P53" s="20"/>
-      <c r="Q53" s="20"/>
-      <c r="R53" s="20"/>
-      <c r="S53" s="20"/>
-      <c r="T53" s="20"/>
-      <c r="U53" s="20"/>
-      <c r="V53" s="20"/>
-      <c r="W53" s="20"/>
-      <c r="X53" s="20"/>
-      <c r="Y53" s="20"/>
-      <c r="Z53" s="20"/>
-      <c r="AA53" s="20"/>
-      <c r="AB53" s="20"/>
-      <c r="AC53" s="20"/>
-      <c r="AD53" s="20"/>
-      <c r="AE53" s="20"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B53" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="C53" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="P54" s="0" t="s">
+      <c r="P53" s="0" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="19" t="s">
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B55" s="19"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="20"/>
-      <c r="G55" s="20"/>
-      <c r="H55" s="20"/>
-      <c r="I55" s="20"/>
-      <c r="J55" s="20"/>
-      <c r="K55" s="20"/>
-      <c r="L55" s="20"/>
-      <c r="M55" s="20"/>
-      <c r="N55" s="20"/>
-      <c r="O55" s="20"/>
-      <c r="P55" s="20"/>
-      <c r="Q55" s="20"/>
-      <c r="R55" s="20"/>
-      <c r="S55" s="20"/>
-      <c r="T55" s="20"/>
-      <c r="U55" s="20"/>
-      <c r="V55" s="20"/>
-      <c r="W55" s="20"/>
-      <c r="X55" s="20"/>
-      <c r="Y55" s="20"/>
-      <c r="Z55" s="20"/>
-      <c r="AA55" s="20"/>
-      <c r="AB55" s="20"/>
-      <c r="AC55" s="20"/>
-      <c r="AD55" s="20"/>
-      <c r="AE55" s="20"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="20"/>
+      <c r="H54" s="20"/>
+      <c r="I54" s="20"/>
+      <c r="J54" s="20"/>
+      <c r="K54" s="20"/>
+      <c r="L54" s="20"/>
+      <c r="M54" s="20"/>
+      <c r="N54" s="20"/>
+      <c r="O54" s="20"/>
+      <c r="P54" s="20"/>
+      <c r="Q54" s="20"/>
+      <c r="R54" s="20"/>
+      <c r="S54" s="20"/>
+      <c r="T54" s="20"/>
+      <c r="U54" s="20"/>
+      <c r="V54" s="20"/>
+      <c r="W54" s="20"/>
+      <c r="X54" s="20"/>
+      <c r="Y54" s="20"/>
+      <c r="Z54" s="20"/>
+      <c r="AA54" s="20"/>
+      <c r="AB54" s="20"/>
+      <c r="AC54" s="20"/>
+      <c r="AD54" s="20"/>
+      <c r="AE54" s="20"/>
+    </row>
+    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B55" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C55" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D55" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="E55" s="25"/>
+      <c r="F55" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="G55" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="H55" s="26"/>
+      <c r="I55" s="26"/>
+      <c r="J55" s="26"/>
+      <c r="K55" s="27"/>
+      <c r="L55" s="26"/>
+      <c r="M55" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="N55" s="26"/>
+      <c r="O55" s="26"/>
+      <c r="P55" s="29"/>
+      <c r="Q55" s="29"/>
+      <c r="R55" s="29"/>
+      <c r="S55" s="29"/>
+      <c r="T55" s="29"/>
+      <c r="U55" s="29"/>
+      <c r="V55" s="29"/>
+      <c r="W55" s="29"/>
+      <c r="X55" s="29"/>
+      <c r="Y55" s="29"/>
+      <c r="Z55" s="29"/>
+      <c r="AA55" s="30"/>
+      <c r="AB55" s="30"/>
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B56" s="22" t="s">
-        <v>115</v>
+      <c r="A56" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B56" s="31" t="s">
+        <v>117</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>31</v>
+        <v>118</v>
       </c>
       <c r="D56" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="E56" s="25"/>
-      <c r="F56" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="G56" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="H56" s="26"/>
-      <c r="I56" s="26"/>
-      <c r="J56" s="26"/>
+        <v>119</v>
+      </c>
+      <c r="E56" s="31"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="H56" s="32"/>
+      <c r="I56" s="32"/>
+      <c r="J56" s="32"/>
       <c r="K56" s="27"/>
-      <c r="L56" s="26"/>
-      <c r="M56" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="N56" s="26"/>
-      <c r="O56" s="26"/>
-      <c r="P56" s="29"/>
-      <c r="Q56" s="29"/>
-      <c r="R56" s="29"/>
-      <c r="S56" s="29"/>
-      <c r="T56" s="29"/>
-      <c r="U56" s="29"/>
-      <c r="V56" s="29"/>
-      <c r="W56" s="29"/>
-      <c r="X56" s="29"/>
-      <c r="Y56" s="29"/>
-      <c r="Z56" s="29"/>
+      <c r="L56" s="32"/>
+      <c r="M56" s="32"/>
+      <c r="N56" s="32"/>
+      <c r="O56" s="32"/>
+      <c r="P56" s="32"/>
+      <c r="Q56" s="32"/>
+      <c r="R56" s="32"/>
+      <c r="S56" s="32"/>
+      <c r="T56" s="32"/>
+      <c r="U56" s="32"/>
+      <c r="V56" s="32"/>
+      <c r="W56" s="32"/>
+      <c r="X56" s="32"/>
+      <c r="Y56" s="32"/>
+      <c r="Z56" s="32"/>
       <c r="AA56" s="30"/>
       <c r="AB56" s="30"/>
     </row>
-    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="31" t="s">
+    <row r="57" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="B57" s="31" t="s">
-        <v>117</v>
+      <c r="B57" s="33" t="s">
+        <v>121</v>
       </c>
       <c r="C57" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="D57" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="E57" s="31"/>
-      <c r="F57" s="32"/>
-      <c r="G57" s="31" t="s">
-        <v>120</v>
+        <v>122</v>
+      </c>
+      <c r="D57" s="24"/>
+      <c r="E57" s="33"/>
+      <c r="F57" s="34"/>
+      <c r="G57" s="22" t="s">
+        <v>123</v>
       </c>
       <c r="H57" s="32"/>
       <c r="I57" s="32"/>
@@ -3422,16 +3460,18 @@
         <v>101</v>
       </c>
       <c r="B58" s="33" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C58" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="D58" s="24"/>
+        <v>125</v>
+      </c>
+      <c r="D58" s="24" t="s">
+        <v>126</v>
+      </c>
       <c r="E58" s="33"/>
       <c r="F58" s="34"/>
-      <c r="G58" s="22" t="s">
-        <v>123</v>
+      <c r="G58" s="33" t="s">
+        <v>127</v>
       </c>
       <c r="H58" s="32"/>
       <c r="I58" s="32"/>
@@ -3460,18 +3500,16 @@
         <v>101</v>
       </c>
       <c r="B59" s="33" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C59" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="D59" s="24" t="s">
-        <v>126</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="D59" s="24"/>
       <c r="E59" s="33"/>
       <c r="F59" s="34"/>
-      <c r="G59" s="33" t="s">
-        <v>127</v>
+      <c r="G59" s="22" t="s">
+        <v>123</v>
       </c>
       <c r="H59" s="32"/>
       <c r="I59" s="32"/>
@@ -3500,10 +3538,10 @@
         <v>101</v>
       </c>
       <c r="B60" s="33" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C60" s="23" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D60" s="24"/>
       <c r="E60" s="33"/>
@@ -3537,17 +3575,17 @@
       <c r="A61" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="B61" s="33" t="s">
-        <v>130</v>
+      <c r="B61" s="22" t="s">
+        <v>132</v>
       </c>
       <c r="C61" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="D61" s="24"/>
-      <c r="E61" s="33"/>
-      <c r="F61" s="34"/>
+        <v>133</v>
+      </c>
+      <c r="D61" s="22"/>
+      <c r="E61" s="22"/>
+      <c r="F61" s="25"/>
       <c r="G61" s="22" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="H61" s="32"/>
       <c r="I61" s="32"/>
@@ -3576,16 +3614,18 @@
         <v>101</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C62" s="23" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D62" s="22"/>
       <c r="E62" s="22"/>
-      <c r="F62" s="25"/>
+      <c r="F62" s="25" t="s">
+        <v>137</v>
+      </c>
       <c r="G62" s="22" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="H62" s="32"/>
       <c r="I62" s="32"/>
@@ -3614,15 +3654,15 @@
         <v>101</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C63" s="23" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D63" s="22"/>
       <c r="E63" s="22"/>
       <c r="F63" s="25" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G63" s="22" t="s">
         <v>123</v>
@@ -3654,15 +3694,15 @@
         <v>101</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C64" s="23" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D64" s="22"/>
       <c r="E64" s="22"/>
       <c r="F64" s="25" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="G64" s="22" t="s">
         <v>123</v>
@@ -3694,18 +3734,18 @@
         <v>101</v>
       </c>
       <c r="B65" s="22" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C65" s="23" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D65" s="22"/>
       <c r="E65" s="22"/>
       <c r="F65" s="25" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G65" s="22" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="H65" s="32"/>
       <c r="I65" s="32"/>
@@ -3734,18 +3774,16 @@
         <v>101</v>
       </c>
       <c r="B66" s="22" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C66" s="23" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D66" s="22"/>
       <c r="E66" s="22"/>
-      <c r="F66" s="25" t="s">
-        <v>140</v>
-      </c>
+      <c r="F66" s="25"/>
       <c r="G66" s="22" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="H66" s="32"/>
       <c r="I66" s="32"/>
@@ -3774,16 +3812,16 @@
         <v>101</v>
       </c>
       <c r="B67" s="22" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C67" s="23" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D67" s="22"/>
       <c r="E67" s="22"/>
       <c r="F67" s="25"/>
       <c r="G67" s="22" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="H67" s="32"/>
       <c r="I67" s="32"/>
@@ -3807,73 +3845,35 @@
       <c r="AA67" s="30"/>
       <c r="AB67" s="30"/>
     </row>
-    <row r="68" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="B68" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="C68" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="D68" s="22"/>
-      <c r="E68" s="22"/>
-      <c r="F68" s="25"/>
-      <c r="G68" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="H68" s="32"/>
-      <c r="I68" s="32"/>
+    <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="H68" s="29"/>
+      <c r="I68" s="29"/>
       <c r="J68" s="32"/>
       <c r="K68" s="27"/>
-      <c r="L68" s="32"/>
-      <c r="M68" s="32"/>
-      <c r="N68" s="32"/>
-      <c r="O68" s="32"/>
-      <c r="P68" s="32"/>
-      <c r="Q68" s="32"/>
-      <c r="R68" s="32"/>
-      <c r="S68" s="32"/>
-      <c r="T68" s="32"/>
-      <c r="U68" s="32"/>
-      <c r="V68" s="32"/>
-      <c r="W68" s="32"/>
-      <c r="X68" s="32"/>
-      <c r="Y68" s="32"/>
-      <c r="Z68" s="32"/>
+      <c r="L68" s="29"/>
+      <c r="M68" s="29"/>
+      <c r="N68" s="29"/>
+      <c r="O68" s="29"/>
+      <c r="P68" s="29"/>
+      <c r="Q68" s="29"/>
+      <c r="R68" s="29"/>
+      <c r="S68" s="29"/>
+      <c r="T68" s="29"/>
+      <c r="U68" s="29"/>
+      <c r="V68" s="29"/>
+      <c r="W68" s="29"/>
+      <c r="X68" s="29"/>
+      <c r="Y68" s="29"/>
+      <c r="Z68" s="29"/>
       <c r="AA68" s="30"/>
       <c r="AB68" s="30"/>
     </row>
-    <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="H69" s="29"/>
-      <c r="I69" s="29"/>
-      <c r="J69" s="32"/>
-      <c r="K69" s="27"/>
-      <c r="L69" s="29"/>
-      <c r="M69" s="29"/>
-      <c r="N69" s="29"/>
-      <c r="O69" s="29"/>
-      <c r="P69" s="29"/>
-      <c r="Q69" s="29"/>
-      <c r="R69" s="29"/>
-      <c r="S69" s="29"/>
-      <c r="T69" s="29"/>
-      <c r="U69" s="29"/>
-      <c r="V69" s="29"/>
-      <c r="W69" s="29"/>
-      <c r="X69" s="29"/>
-      <c r="Y69" s="29"/>
-      <c r="Z69" s="29"/>
-      <c r="AA69" s="30"/>
-      <c r="AB69" s="30"/>
-    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E48:E53 E55" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E47:E52 E54" type="list">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3907,7 +3907,7 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.59765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.61328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="2" style="35" width="45.84"/>
@@ -4148,7 +4148,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.83"/>
@@ -4205,7 +4205,7 @@
       </c>
       <c r="C2" s="49" t="n">
         <f aca="true">NOW()</f>
-        <v>45113.8452357324</v>
+        <v>45138.6238921957</v>
       </c>
       <c r="D2" s="50" t="s">
         <v>171</v>

</xml_diff>

<commit_message>
Updated workflows, forms and condition cards
</commit_message>
<xml_diff>
--- a/POSHIT/Example CHT application/malaria-usecase-cht/forms/app/children_under_5_follow_up.xlsx
+++ b/POSHIT/Example CHT application/malaria-usecase-cht/forms/app/children_under_5_follow_up.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="201">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -309,6 +309,12 @@
     <t xml:space="preserve">selected(${availability}, ‘no’)</t>
   </si>
   <si>
+    <t xml:space="preserve">floor(decimal-date-time(.)) &gt; floor(decimal-date-time(today()))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date cannot be in the past</t>
+  </si>
+  <si>
     <t xml:space="preserve">children_under_5_follow_up</t>
   </si>
   <si>
@@ -318,6 +324,100 @@
     <t xml:space="preserve">selected(${availability}, ‘yes’)</t>
   </si>
   <si>
+    <t xml:space="preserve">go_to_health_facility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Did ${patient_name} go to the health facility as referred?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">select_multiple </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">reason_not_go_facility</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">reason_not_go_facility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Why did ${patient_name} not go to the health facility as referred?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(${go_to_health_facility},’no’)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specify_other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specify Other</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">selected(${</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">reason_not_go_facility},’other’)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">further_check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encourage ${patient_name} to go to the health facility for further management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_of_facility_visit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date when ${patient_name} will go to the health facility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tests_done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Were there tests done?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(${go_to_health_facility},’yes’)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">malaria_confirmed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was malaria confirmed?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(${tests_done},’yes’)</t>
+  </si>
+  <si>
     <t xml:space="preserve">select_one child_condition</t>
   </si>
   <si>
@@ -325,9 +425,6 @@
   </si>
   <si>
     <t xml:space="preserve">How is the child doing?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">note</t>
   </si>
   <si>
     <t xml:space="preserve">improvement_check</t>
@@ -566,6 +663,24 @@
   </si>
   <si>
     <t xml:space="preserve">cured</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lack_of_transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lack of transport fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">felt_better</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Child felt better</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other</t>
   </si>
   <si>
     <t xml:space="preserve">form_title</t>
@@ -849,7 +964,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -926,11 +1041,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1135,13 +1258,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AJ68"/>
+  <dimension ref="A1:AJ75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C67" activeCellId="0" sqref="C67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.55"/>
@@ -3015,7 +3138,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>91</v>
       </c>
@@ -3027,6 +3150,12 @@
       </c>
       <c r="F44" s="0" t="s">
         <v>94</v>
+      </c>
+      <c r="H44" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="I44" s="0" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3035,845 +3164,1142 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B47" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
+      <c r="B47" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
       <c r="F47" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="G47" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="G47" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
-      <c r="J47" s="20"/>
-      <c r="K47" s="20"/>
-      <c r="L47" s="20"/>
-      <c r="M47" s="20"/>
-      <c r="N47" s="20"/>
-      <c r="O47" s="20"/>
-      <c r="P47" s="20"/>
-      <c r="Q47" s="20"/>
-      <c r="R47" s="20"/>
-      <c r="S47" s="20"/>
-      <c r="T47" s="20"/>
-      <c r="U47" s="20"/>
-      <c r="V47" s="20"/>
-      <c r="W47" s="20"/>
-      <c r="X47" s="20"/>
-      <c r="Y47" s="20"/>
-      <c r="Z47" s="20"/>
-      <c r="AA47" s="20"/>
-      <c r="AB47" s="20"/>
-      <c r="AC47" s="20"/>
-      <c r="AD47" s="20"/>
-      <c r="AE47" s="20"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
+      <c r="J47" s="21"/>
+      <c r="K47" s="21"/>
+      <c r="L47" s="21"/>
+      <c r="M47" s="21"/>
+      <c r="N47" s="21"/>
+      <c r="O47" s="21"/>
+      <c r="P47" s="21"/>
+      <c r="Q47" s="21"/>
+      <c r="R47" s="21"/>
+      <c r="S47" s="21"/>
+      <c r="T47" s="21"/>
+      <c r="U47" s="21"/>
+      <c r="V47" s="21"/>
+      <c r="W47" s="21"/>
+      <c r="X47" s="21"/>
+      <c r="Y47" s="21"/>
+      <c r="Z47" s="21"/>
+      <c r="AA47" s="21"/>
+      <c r="AB47" s="21"/>
+      <c r="AC47" s="21"/>
+      <c r="AD47" s="21"/>
+      <c r="AE47" s="21"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="B48" s="19" t="s">
+      <c r="A48" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="21"/>
+      <c r="J48" s="21"/>
+      <c r="K48" s="21"/>
+      <c r="L48" s="21"/>
+      <c r="M48" s="21"/>
+      <c r="N48" s="21"/>
+      <c r="O48" s="21"/>
+      <c r="P48" s="21"/>
+      <c r="Q48" s="21"/>
+      <c r="R48" s="21"/>
+      <c r="S48" s="21"/>
+      <c r="T48" s="21"/>
+      <c r="U48" s="21"/>
+      <c r="V48" s="21"/>
+      <c r="W48" s="21"/>
+      <c r="X48" s="21"/>
+      <c r="Y48" s="21"/>
+      <c r="Z48" s="21"/>
+      <c r="AA48" s="21"/>
+      <c r="AB48" s="21"/>
+      <c r="AC48" s="21"/>
+      <c r="AD48" s="21"/>
+      <c r="AE48" s="21"/>
+    </row>
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="F49" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="21"/>
+      <c r="J49" s="21"/>
+      <c r="K49" s="21"/>
+      <c r="L49" s="21"/>
+      <c r="M49" s="21"/>
+      <c r="N49" s="21"/>
+      <c r="O49" s="21"/>
+      <c r="P49" s="21"/>
+      <c r="Q49" s="21"/>
+      <c r="R49" s="21"/>
+      <c r="S49" s="21"/>
+      <c r="T49" s="21"/>
+      <c r="U49" s="21"/>
+      <c r="V49" s="21"/>
+      <c r="W49" s="21"/>
+      <c r="X49" s="21"/>
+      <c r="Y49" s="21"/>
+      <c r="Z49" s="21"/>
+      <c r="AA49" s="21"/>
+      <c r="AB49" s="21"/>
+      <c r="AC49" s="21"/>
+      <c r="AD49" s="21"/>
+      <c r="AE49" s="21"/>
+    </row>
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="F50" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="21"/>
+      <c r="J50" s="21"/>
+      <c r="K50" s="21"/>
+      <c r="L50" s="21"/>
+      <c r="M50" s="21"/>
+      <c r="N50" s="21"/>
+      <c r="O50" s="21"/>
+      <c r="P50" s="21"/>
+      <c r="Q50" s="21"/>
+      <c r="R50" s="21"/>
+      <c r="S50" s="21"/>
+      <c r="T50" s="21"/>
+      <c r="U50" s="21"/>
+      <c r="V50" s="21"/>
+      <c r="W50" s="21"/>
+      <c r="X50" s="21"/>
+      <c r="Y50" s="21"/>
+      <c r="Z50" s="21"/>
+      <c r="AA50" s="21"/>
+      <c r="AB50" s="21"/>
+      <c r="AC50" s="21"/>
+      <c r="AD50" s="21"/>
+      <c r="AE50" s="21"/>
+    </row>
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="G51" s="21"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="21"/>
+      <c r="J51" s="21"/>
+      <c r="K51" s="21"/>
+      <c r="L51" s="21"/>
+      <c r="M51" s="21"/>
+      <c r="N51" s="21"/>
+      <c r="O51" s="21"/>
+      <c r="P51" s="21"/>
+      <c r="Q51" s="21"/>
+      <c r="R51" s="21"/>
+      <c r="S51" s="21"/>
+      <c r="T51" s="21"/>
+      <c r="U51" s="21"/>
+      <c r="V51" s="21"/>
+      <c r="W51" s="21"/>
+      <c r="X51" s="21"/>
+      <c r="Y51" s="21"/>
+      <c r="Z51" s="21"/>
+      <c r="AA51" s="21"/>
+      <c r="AB51" s="21"/>
+      <c r="AC51" s="21"/>
+      <c r="AD51" s="21"/>
+      <c r="AE51" s="21"/>
+    </row>
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B52" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C52" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="F52" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="G52" s="21"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="21"/>
+      <c r="J52" s="21"/>
+      <c r="K52" s="21"/>
+      <c r="L52" s="21"/>
+      <c r="M52" s="21"/>
+      <c r="N52" s="21"/>
+      <c r="O52" s="21"/>
+      <c r="P52" s="21"/>
+      <c r="Q52" s="21"/>
+      <c r="R52" s="21"/>
+      <c r="S52" s="21"/>
+      <c r="T52" s="21"/>
+      <c r="U52" s="21"/>
+      <c r="V52" s="21"/>
+      <c r="W52" s="21"/>
+      <c r="X52" s="21"/>
+      <c r="Y52" s="21"/>
+      <c r="Z52" s="21"/>
+      <c r="AA52" s="21"/>
+      <c r="AB52" s="21"/>
+      <c r="AC52" s="21"/>
+      <c r="AD52" s="21"/>
+      <c r="AE52" s="21"/>
+    </row>
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B53" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="F53" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="G53" s="21"/>
+      <c r="H53" s="21"/>
+      <c r="I53" s="21"/>
+      <c r="J53" s="21"/>
+      <c r="K53" s="21"/>
+      <c r="L53" s="21"/>
+      <c r="M53" s="21"/>
+      <c r="N53" s="21"/>
+      <c r="O53" s="21"/>
+      <c r="P53" s="21"/>
+      <c r="Q53" s="21"/>
+      <c r="R53" s="21"/>
+      <c r="S53" s="21"/>
+      <c r="T53" s="21"/>
+      <c r="U53" s="21"/>
+      <c r="V53" s="21"/>
+      <c r="W53" s="21"/>
+      <c r="X53" s="21"/>
+      <c r="Y53" s="21"/>
+      <c r="Z53" s="21"/>
+      <c r="AA53" s="21"/>
+      <c r="AB53" s="21"/>
+      <c r="AC53" s="21"/>
+      <c r="AD53" s="21"/>
+      <c r="AE53" s="21"/>
+    </row>
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B54" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="F54" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="G54" s="21"/>
+      <c r="H54" s="21"/>
+      <c r="I54" s="21"/>
+      <c r="J54" s="21"/>
+      <c r="K54" s="21"/>
+      <c r="L54" s="21"/>
+      <c r="M54" s="21"/>
+      <c r="N54" s="21"/>
+      <c r="O54" s="21"/>
+      <c r="P54" s="21"/>
+      <c r="Q54" s="21"/>
+      <c r="R54" s="21"/>
+      <c r="S54" s="21"/>
+      <c r="T54" s="21"/>
+      <c r="U54" s="21"/>
+      <c r="V54" s="21"/>
+      <c r="W54" s="21"/>
+      <c r="X54" s="21"/>
+      <c r="Y54" s="21"/>
+      <c r="Z54" s="21"/>
+      <c r="AA54" s="21"/>
+      <c r="AB54" s="21"/>
+      <c r="AC54" s="21"/>
+      <c r="AD54" s="21"/>
+      <c r="AE54" s="21"/>
+    </row>
+    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B55" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="C55" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="D55" s="21"/>
+      <c r="E55" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="F55" s="21"/>
+      <c r="G55" s="21"/>
+      <c r="H55" s="21"/>
+      <c r="I55" s="21"/>
+      <c r="J55" s="21"/>
+      <c r="K55" s="21"/>
+      <c r="L55" s="21"/>
+      <c r="M55" s="21"/>
+      <c r="N55" s="21"/>
+      <c r="O55" s="21"/>
+      <c r="P55" s="21"/>
+      <c r="Q55" s="21"/>
+      <c r="R55" s="21"/>
+      <c r="S55" s="21"/>
+      <c r="T55" s="21"/>
+      <c r="U55" s="21"/>
+      <c r="V55" s="21"/>
+      <c r="W55" s="21"/>
+      <c r="X55" s="21"/>
+      <c r="Y55" s="21"/>
+      <c r="Z55" s="21"/>
+      <c r="AA55" s="21"/>
+      <c r="AB55" s="21"/>
+      <c r="AC55" s="21"/>
+      <c r="AD55" s="21"/>
+      <c r="AE55" s="21"/>
+    </row>
+    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B56" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="C56" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="G56" s="21"/>
+      <c r="H56" s="21"/>
+      <c r="I56" s="21"/>
+      <c r="J56" s="21"/>
+      <c r="K56" s="21"/>
+      <c r="L56" s="21"/>
+      <c r="M56" s="21"/>
+      <c r="N56" s="21"/>
+      <c r="O56" s="21"/>
+      <c r="P56" s="21"/>
+      <c r="Q56" s="21"/>
+      <c r="R56" s="21"/>
+      <c r="S56" s="21"/>
+      <c r="T56" s="21"/>
+      <c r="U56" s="21"/>
+      <c r="V56" s="21"/>
+      <c r="W56" s="21"/>
+      <c r="X56" s="21"/>
+      <c r="Y56" s="21"/>
+      <c r="Z56" s="21"/>
+      <c r="AA56" s="21"/>
+      <c r="AB56" s="21"/>
+      <c r="AC56" s="21"/>
+      <c r="AD56" s="21"/>
+      <c r="AE56" s="21"/>
+    </row>
+    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B57" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="C57" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="G57" s="21"/>
+      <c r="H57" s="21"/>
+      <c r="I57" s="21"/>
+      <c r="J57" s="21"/>
+      <c r="K57" s="21"/>
+      <c r="L57" s="21"/>
+      <c r="M57" s="21"/>
+      <c r="N57" s="21"/>
+      <c r="O57" s="21"/>
+      <c r="P57" s="21"/>
+      <c r="Q57" s="21"/>
+      <c r="R57" s="21"/>
+      <c r="S57" s="21"/>
+      <c r="T57" s="21"/>
+      <c r="U57" s="21"/>
+      <c r="V57" s="21"/>
+      <c r="W57" s="21"/>
+      <c r="X57" s="21"/>
+      <c r="Y57" s="21"/>
+      <c r="Z57" s="21"/>
+      <c r="AA57" s="21"/>
+      <c r="AB57" s="21"/>
+      <c r="AC57" s="21"/>
+      <c r="AD57" s="21"/>
+      <c r="AE57" s="21"/>
+    </row>
+    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B58" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="C58" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="G58" s="21"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21"/>
+      <c r="J58" s="21"/>
+      <c r="K58" s="21"/>
+      <c r="L58" s="21"/>
+      <c r="M58" s="21"/>
+      <c r="N58" s="21"/>
+      <c r="O58" s="21"/>
+      <c r="P58" s="21"/>
+      <c r="Q58" s="21"/>
+      <c r="R58" s="21"/>
+      <c r="S58" s="21"/>
+      <c r="T58" s="21"/>
+      <c r="U58" s="21"/>
+      <c r="V58" s="21"/>
+      <c r="W58" s="21"/>
+      <c r="X58" s="21"/>
+      <c r="Y58" s="21"/>
+      <c r="Z58" s="21"/>
+      <c r="AA58" s="21"/>
+      <c r="AB58" s="21"/>
+      <c r="AC58" s="21"/>
+      <c r="AD58" s="21"/>
+      <c r="AE58" s="21"/>
+    </row>
+    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B59" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="C59" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="F59" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="G59" s="21"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="21"/>
+      <c r="J59" s="21"/>
+      <c r="K59" s="21"/>
+      <c r="L59" s="21"/>
+      <c r="M59" s="21"/>
+      <c r="N59" s="21"/>
+      <c r="O59" s="21"/>
+      <c r="P59" s="21"/>
+      <c r="Q59" s="21"/>
+      <c r="R59" s="21"/>
+      <c r="S59" s="21"/>
+      <c r="T59" s="21"/>
+      <c r="U59" s="21"/>
+      <c r="V59" s="21"/>
+      <c r="W59" s="21"/>
+      <c r="X59" s="21"/>
+      <c r="Y59" s="21"/>
+      <c r="Z59" s="21"/>
+      <c r="AA59" s="21"/>
+      <c r="AB59" s="21"/>
+      <c r="AC59" s="21"/>
+      <c r="AD59" s="21"/>
+      <c r="AE59" s="21"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P60" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B61" s="20"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="21"/>
+      <c r="G61" s="21"/>
+      <c r="H61" s="21"/>
+      <c r="I61" s="21"/>
+      <c r="J61" s="21"/>
+      <c r="K61" s="21"/>
+      <c r="L61" s="21"/>
+      <c r="M61" s="21"/>
+      <c r="N61" s="21"/>
+      <c r="O61" s="21"/>
+      <c r="P61" s="21"/>
+      <c r="Q61" s="21"/>
+      <c r="R61" s="21"/>
+      <c r="S61" s="21"/>
+      <c r="T61" s="21"/>
+      <c r="U61" s="21"/>
+      <c r="V61" s="21"/>
+      <c r="W61" s="21"/>
+      <c r="X61" s="21"/>
+      <c r="Y61" s="21"/>
+      <c r="Z61" s="21"/>
+      <c r="AA61" s="21"/>
+      <c r="AB61" s="21"/>
+      <c r="AC61" s="21"/>
+      <c r="AD61" s="21"/>
+      <c r="AE61" s="21"/>
+    </row>
+    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B62" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="C62" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E62" s="27"/>
+      <c r="F62" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="C48" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="F48" s="20"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="20"/>
-      <c r="I48" s="20"/>
-      <c r="J48" s="20"/>
-      <c r="K48" s="20"/>
-      <c r="L48" s="20"/>
-      <c r="M48" s="20"/>
-      <c r="N48" s="20"/>
-      <c r="O48" s="20"/>
-      <c r="P48" s="20"/>
-      <c r="Q48" s="20"/>
-      <c r="R48" s="20"/>
-      <c r="S48" s="20"/>
-      <c r="T48" s="20"/>
-      <c r="U48" s="20"/>
-      <c r="V48" s="20"/>
-      <c r="W48" s="20"/>
-      <c r="X48" s="20"/>
-      <c r="Y48" s="20"/>
-      <c r="Z48" s="20"/>
-      <c r="AA48" s="20"/>
-      <c r="AB48" s="20"/>
-      <c r="AC48" s="20"/>
-      <c r="AD48" s="20"/>
-      <c r="AE48" s="20"/>
-    </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="B49" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="C49" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="G49" s="20"/>
-      <c r="H49" s="20"/>
-      <c r="I49" s="20"/>
-      <c r="J49" s="20"/>
-      <c r="K49" s="20"/>
-      <c r="L49" s="20"/>
-      <c r="M49" s="20"/>
-      <c r="N49" s="20"/>
-      <c r="O49" s="20"/>
-      <c r="P49" s="20"/>
-      <c r="Q49" s="20"/>
-      <c r="R49" s="20"/>
-      <c r="S49" s="20"/>
-      <c r="T49" s="20"/>
-      <c r="U49" s="20"/>
-      <c r="V49" s="20"/>
-      <c r="W49" s="20"/>
-      <c r="X49" s="20"/>
-      <c r="Y49" s="20"/>
-      <c r="Z49" s="20"/>
-      <c r="AA49" s="20"/>
-      <c r="AB49" s="20"/>
-      <c r="AC49" s="20"/>
-      <c r="AD49" s="20"/>
-      <c r="AE49" s="20"/>
-    </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="B50" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="C50" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="G50" s="20"/>
-      <c r="H50" s="20"/>
-      <c r="I50" s="20"/>
-      <c r="J50" s="20"/>
-      <c r="K50" s="20"/>
-      <c r="L50" s="20"/>
-      <c r="M50" s="20"/>
-      <c r="N50" s="20"/>
-      <c r="O50" s="20"/>
-      <c r="P50" s="20"/>
-      <c r="Q50" s="20"/>
-      <c r="R50" s="20"/>
-      <c r="S50" s="20"/>
-      <c r="T50" s="20"/>
-      <c r="U50" s="20"/>
-      <c r="V50" s="20"/>
-      <c r="W50" s="20"/>
-      <c r="X50" s="20"/>
-      <c r="Y50" s="20"/>
-      <c r="Z50" s="20"/>
-      <c r="AA50" s="20"/>
-      <c r="AB50" s="20"/>
-      <c r="AC50" s="20"/>
-      <c r="AD50" s="20"/>
-      <c r="AE50" s="20"/>
-    </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="B51" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="C51" s="20" t="s">
+      <c r="G62" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="H62" s="28"/>
+      <c r="I62" s="28"/>
+      <c r="J62" s="28"/>
+      <c r="K62" s="29"/>
+      <c r="L62" s="28"/>
+      <c r="M62" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="N62" s="28"/>
+      <c r="O62" s="28"/>
+      <c r="P62" s="31"/>
+      <c r="Q62" s="31"/>
+      <c r="R62" s="31"/>
+      <c r="S62" s="31"/>
+      <c r="T62" s="31"/>
+      <c r="U62" s="31"/>
+      <c r="V62" s="31"/>
+      <c r="W62" s="31"/>
+      <c r="X62" s="31"/>
+      <c r="Y62" s="31"/>
+      <c r="Z62" s="31"/>
+      <c r="AA62" s="32"/>
+      <c r="AB62" s="32"/>
+    </row>
+    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
-      <c r="I51" s="20"/>
-      <c r="J51" s="20"/>
-      <c r="K51" s="20"/>
-      <c r="L51" s="20"/>
-      <c r="M51" s="20"/>
-      <c r="N51" s="20"/>
-      <c r="O51" s="20"/>
-      <c r="P51" s="20"/>
-      <c r="Q51" s="20"/>
-      <c r="R51" s="20"/>
-      <c r="S51" s="20"/>
-      <c r="T51" s="20"/>
-      <c r="U51" s="20"/>
-      <c r="V51" s="20"/>
-      <c r="W51" s="20"/>
-      <c r="X51" s="20"/>
-      <c r="Y51" s="20"/>
-      <c r="Z51" s="20"/>
-      <c r="AA51" s="20"/>
-      <c r="AB51" s="20"/>
-      <c r="AC51" s="20"/>
-      <c r="AD51" s="20"/>
-      <c r="AE51" s="20"/>
-    </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="B52" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="C52" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="F52" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="G52" s="20"/>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20"/>
-      <c r="J52" s="20"/>
-      <c r="K52" s="20"/>
-      <c r="L52" s="20"/>
-      <c r="M52" s="20"/>
-      <c r="N52" s="20"/>
-      <c r="O52" s="20"/>
-      <c r="P52" s="20"/>
-      <c r="Q52" s="20"/>
-      <c r="R52" s="20"/>
-      <c r="S52" s="20"/>
-      <c r="T52" s="20"/>
-      <c r="U52" s="20"/>
-      <c r="V52" s="20"/>
-      <c r="W52" s="20"/>
-      <c r="X52" s="20"/>
-      <c r="Y52" s="20"/>
-      <c r="Z52" s="20"/>
-      <c r="AA52" s="20"/>
-      <c r="AB52" s="20"/>
-      <c r="AC52" s="20"/>
-      <c r="AD52" s="20"/>
-      <c r="AE52" s="20"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B53" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="P53" s="0" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="19" t="s">
+      <c r="B63" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="C63" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="D63" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="E63" s="33"/>
+      <c r="F63" s="34"/>
+      <c r="G63" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="H63" s="34"/>
+      <c r="I63" s="34"/>
+      <c r="J63" s="34"/>
+      <c r="K63" s="29"/>
+      <c r="L63" s="34"/>
+      <c r="M63" s="34"/>
+      <c r="N63" s="34"/>
+      <c r="O63" s="34"/>
+      <c r="P63" s="34"/>
+      <c r="Q63" s="34"/>
+      <c r="R63" s="34"/>
+      <c r="S63" s="34"/>
+      <c r="T63" s="34"/>
+      <c r="U63" s="34"/>
+      <c r="V63" s="34"/>
+      <c r="W63" s="34"/>
+      <c r="X63" s="34"/>
+      <c r="Y63" s="34"/>
+      <c r="Z63" s="34"/>
+      <c r="AA63" s="32"/>
+      <c r="AB63" s="32"/>
+    </row>
+    <row r="64" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B64" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="C64" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="D64" s="26"/>
+      <c r="E64" s="35"/>
+      <c r="F64" s="36"/>
+      <c r="G64" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="H64" s="34"/>
+      <c r="I64" s="34"/>
+      <c r="J64" s="34"/>
+      <c r="K64" s="29"/>
+      <c r="L64" s="34"/>
+      <c r="M64" s="34"/>
+      <c r="N64" s="34"/>
+      <c r="O64" s="34"/>
+      <c r="P64" s="34"/>
+      <c r="Q64" s="34"/>
+      <c r="R64" s="34"/>
+      <c r="S64" s="34"/>
+      <c r="T64" s="34"/>
+      <c r="U64" s="34"/>
+      <c r="V64" s="34"/>
+      <c r="W64" s="34"/>
+      <c r="X64" s="34"/>
+      <c r="Y64" s="34"/>
+      <c r="Z64" s="34"/>
+      <c r="AA64" s="32"/>
+      <c r="AB64" s="32"/>
+    </row>
+    <row r="65" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B65" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="C65" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="D65" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="E65" s="35"/>
+      <c r="F65" s="36"/>
+      <c r="G65" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="H65" s="34"/>
+      <c r="I65" s="34"/>
+      <c r="J65" s="34"/>
+      <c r="K65" s="29"/>
+      <c r="L65" s="34"/>
+      <c r="M65" s="34"/>
+      <c r="N65" s="34"/>
+      <c r="O65" s="34"/>
+      <c r="P65" s="34"/>
+      <c r="Q65" s="34"/>
+      <c r="R65" s="34"/>
+      <c r="S65" s="34"/>
+      <c r="T65" s="34"/>
+      <c r="U65" s="34"/>
+      <c r="V65" s="34"/>
+      <c r="W65" s="34"/>
+      <c r="X65" s="34"/>
+      <c r="Y65" s="34"/>
+      <c r="Z65" s="34"/>
+      <c r="AA65" s="32"/>
+      <c r="AB65" s="32"/>
+    </row>
+    <row r="66" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B66" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="C66" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="D66" s="26"/>
+      <c r="E66" s="35"/>
+      <c r="F66" s="36"/>
+      <c r="G66" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="H66" s="34"/>
+      <c r="I66" s="34"/>
+      <c r="J66" s="34"/>
+      <c r="K66" s="29"/>
+      <c r="L66" s="34"/>
+      <c r="M66" s="34"/>
+      <c r="N66" s="34"/>
+      <c r="O66" s="34"/>
+      <c r="P66" s="34"/>
+      <c r="Q66" s="34"/>
+      <c r="R66" s="34"/>
+      <c r="S66" s="34"/>
+      <c r="T66" s="34"/>
+      <c r="U66" s="34"/>
+      <c r="V66" s="34"/>
+      <c r="W66" s="34"/>
+      <c r="X66" s="34"/>
+      <c r="Y66" s="34"/>
+      <c r="Z66" s="34"/>
+      <c r="AA66" s="32"/>
+      <c r="AB66" s="32"/>
+    </row>
+    <row r="67" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B67" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C67" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="D67" s="26"/>
+      <c r="E67" s="35"/>
+      <c r="F67" s="36"/>
+      <c r="G67" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="H67" s="34"/>
+      <c r="I67" s="34"/>
+      <c r="J67" s="34"/>
+      <c r="K67" s="29"/>
+      <c r="L67" s="34"/>
+      <c r="M67" s="34"/>
+      <c r="N67" s="34"/>
+      <c r="O67" s="34"/>
+      <c r="P67" s="34"/>
+      <c r="Q67" s="34"/>
+      <c r="R67" s="34"/>
+      <c r="S67" s="34"/>
+      <c r="T67" s="34"/>
+      <c r="U67" s="34"/>
+      <c r="V67" s="34"/>
+      <c r="W67" s="34"/>
+      <c r="X67" s="34"/>
+      <c r="Y67" s="34"/>
+      <c r="Z67" s="34"/>
+      <c r="AA67" s="32"/>
+      <c r="AB67" s="32"/>
+    </row>
+    <row r="68" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B68" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="C68" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="D68" s="24"/>
+      <c r="E68" s="24"/>
+      <c r="F68" s="27"/>
+      <c r="G68" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="H68" s="34"/>
+      <c r="I68" s="34"/>
+      <c r="J68" s="34"/>
+      <c r="K68" s="29"/>
+      <c r="L68" s="34"/>
+      <c r="M68" s="34"/>
+      <c r="N68" s="34"/>
+      <c r="O68" s="34"/>
+      <c r="P68" s="34"/>
+      <c r="Q68" s="34"/>
+      <c r="R68" s="34"/>
+      <c r="S68" s="34"/>
+      <c r="T68" s="34"/>
+      <c r="U68" s="34"/>
+      <c r="V68" s="34"/>
+      <c r="W68" s="34"/>
+      <c r="X68" s="34"/>
+      <c r="Y68" s="34"/>
+      <c r="Z68" s="34"/>
+      <c r="AA68" s="32"/>
+      <c r="AB68" s="32"/>
+    </row>
+    <row r="69" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B69" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="C69" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="D69" s="24"/>
+      <c r="E69" s="24"/>
+      <c r="F69" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="G69" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="H69" s="34"/>
+      <c r="I69" s="34"/>
+      <c r="J69" s="34"/>
+      <c r="K69" s="29"/>
+      <c r="L69" s="34"/>
+      <c r="M69" s="34"/>
+      <c r="N69" s="34"/>
+      <c r="O69" s="34"/>
+      <c r="P69" s="34"/>
+      <c r="Q69" s="34"/>
+      <c r="R69" s="34"/>
+      <c r="S69" s="34"/>
+      <c r="T69" s="34"/>
+      <c r="U69" s="34"/>
+      <c r="V69" s="34"/>
+      <c r="W69" s="34"/>
+      <c r="X69" s="34"/>
+      <c r="Y69" s="34"/>
+      <c r="Z69" s="34"/>
+      <c r="AA69" s="32"/>
+      <c r="AB69" s="32"/>
+    </row>
+    <row r="70" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B70" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="C70" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D70" s="24"/>
+      <c r="E70" s="24"/>
+      <c r="F70" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="G70" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="H70" s="34"/>
+      <c r="I70" s="34"/>
+      <c r="J70" s="34"/>
+      <c r="K70" s="29"/>
+      <c r="L70" s="34"/>
+      <c r="M70" s="34"/>
+      <c r="N70" s="34"/>
+      <c r="O70" s="34"/>
+      <c r="P70" s="34"/>
+      <c r="Q70" s="34"/>
+      <c r="R70" s="34"/>
+      <c r="S70" s="34"/>
+      <c r="T70" s="34"/>
+      <c r="U70" s="34"/>
+      <c r="V70" s="34"/>
+      <c r="W70" s="34"/>
+      <c r="X70" s="34"/>
+      <c r="Y70" s="34"/>
+      <c r="Z70" s="34"/>
+      <c r="AA70" s="32"/>
+      <c r="AB70" s="32"/>
+    </row>
+    <row r="71" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B71" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="C71" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="D71" s="24"/>
+      <c r="E71" s="24"/>
+      <c r="F71" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="G71" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="H71" s="34"/>
+      <c r="I71" s="34"/>
+      <c r="J71" s="34"/>
+      <c r="K71" s="29"/>
+      <c r="L71" s="34"/>
+      <c r="M71" s="34"/>
+      <c r="N71" s="34"/>
+      <c r="O71" s="34"/>
+      <c r="P71" s="34"/>
+      <c r="Q71" s="34"/>
+      <c r="R71" s="34"/>
+      <c r="S71" s="34"/>
+      <c r="T71" s="34"/>
+      <c r="U71" s="34"/>
+      <c r="V71" s="34"/>
+      <c r="W71" s="34"/>
+      <c r="X71" s="34"/>
+      <c r="Y71" s="34"/>
+      <c r="Z71" s="34"/>
+      <c r="AA71" s="32"/>
+      <c r="AB71" s="32"/>
+    </row>
+    <row r="72" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B72" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="C72" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D72" s="24"/>
+      <c r="E72" s="24"/>
+      <c r="F72" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="G72" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="H72" s="34"/>
+      <c r="I72" s="34"/>
+      <c r="J72" s="34"/>
+      <c r="K72" s="29"/>
+      <c r="L72" s="34"/>
+      <c r="M72" s="34"/>
+      <c r="N72" s="34"/>
+      <c r="O72" s="34"/>
+      <c r="P72" s="34"/>
+      <c r="Q72" s="34"/>
+      <c r="R72" s="34"/>
+      <c r="S72" s="34"/>
+      <c r="T72" s="34"/>
+      <c r="U72" s="34"/>
+      <c r="V72" s="34"/>
+      <c r="W72" s="34"/>
+      <c r="X72" s="34"/>
+      <c r="Y72" s="34"/>
+      <c r="Z72" s="34"/>
+      <c r="AA72" s="32"/>
+      <c r="AB72" s="32"/>
+    </row>
+    <row r="73" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B73" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="C73" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="D73" s="24"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="27"/>
+      <c r="G73" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="H73" s="34"/>
+      <c r="I73" s="34"/>
+      <c r="J73" s="34"/>
+      <c r="K73" s="29"/>
+      <c r="L73" s="34"/>
+      <c r="M73" s="34"/>
+      <c r="N73" s="34"/>
+      <c r="O73" s="34"/>
+      <c r="P73" s="34"/>
+      <c r="Q73" s="34"/>
+      <c r="R73" s="34"/>
+      <c r="S73" s="34"/>
+      <c r="T73" s="34"/>
+      <c r="U73" s="34"/>
+      <c r="V73" s="34"/>
+      <c r="W73" s="34"/>
+      <c r="X73" s="34"/>
+      <c r="Y73" s="34"/>
+      <c r="Z73" s="34"/>
+      <c r="AA73" s="32"/>
+      <c r="AB73" s="32"/>
+    </row>
+    <row r="74" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B74" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="C74" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="D74" s="24"/>
+      <c r="E74" s="24"/>
+      <c r="F74" s="27"/>
+      <c r="G74" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="H74" s="34"/>
+      <c r="I74" s="34"/>
+      <c r="J74" s="34"/>
+      <c r="K74" s="29"/>
+      <c r="L74" s="34"/>
+      <c r="M74" s="34"/>
+      <c r="N74" s="34"/>
+      <c r="O74" s="34"/>
+      <c r="P74" s="34"/>
+      <c r="Q74" s="34"/>
+      <c r="R74" s="34"/>
+      <c r="S74" s="34"/>
+      <c r="T74" s="34"/>
+      <c r="U74" s="34"/>
+      <c r="V74" s="34"/>
+      <c r="W74" s="34"/>
+      <c r="X74" s="34"/>
+      <c r="Y74" s="34"/>
+      <c r="Z74" s="34"/>
+      <c r="AA74" s="32"/>
+      <c r="AB74" s="32"/>
+    </row>
+    <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B54" s="19"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="20"/>
-      <c r="I54" s="20"/>
-      <c r="J54" s="20"/>
-      <c r="K54" s="20"/>
-      <c r="L54" s="20"/>
-      <c r="M54" s="20"/>
-      <c r="N54" s="20"/>
-      <c r="O54" s="20"/>
-      <c r="P54" s="20"/>
-      <c r="Q54" s="20"/>
-      <c r="R54" s="20"/>
-      <c r="S54" s="20"/>
-      <c r="T54" s="20"/>
-      <c r="U54" s="20"/>
-      <c r="V54" s="20"/>
-      <c r="W54" s="20"/>
-      <c r="X54" s="20"/>
-      <c r="Y54" s="20"/>
-      <c r="Z54" s="20"/>
-      <c r="AA54" s="20"/>
-      <c r="AB54" s="20"/>
-      <c r="AC54" s="20"/>
-      <c r="AD54" s="20"/>
-      <c r="AE54" s="20"/>
-    </row>
-    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B55" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="C55" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="D55" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="E55" s="25"/>
-      <c r="F55" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="G55" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="H55" s="26"/>
-      <c r="I55" s="26"/>
-      <c r="J55" s="26"/>
-      <c r="K55" s="27"/>
-      <c r="L55" s="26"/>
-      <c r="M55" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="N55" s="26"/>
-      <c r="O55" s="26"/>
-      <c r="P55" s="29"/>
-      <c r="Q55" s="29"/>
-      <c r="R55" s="29"/>
-      <c r="S55" s="29"/>
-      <c r="T55" s="29"/>
-      <c r="U55" s="29"/>
-      <c r="V55" s="29"/>
-      <c r="W55" s="29"/>
-      <c r="X55" s="29"/>
-      <c r="Y55" s="29"/>
-      <c r="Z55" s="29"/>
-      <c r="AA55" s="30"/>
-      <c r="AB55" s="30"/>
-    </row>
-    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="B56" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="C56" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="D56" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="E56" s="31"/>
-      <c r="F56" s="32"/>
-      <c r="G56" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="H56" s="32"/>
-      <c r="I56" s="32"/>
-      <c r="J56" s="32"/>
-      <c r="K56" s="27"/>
-      <c r="L56" s="32"/>
-      <c r="M56" s="32"/>
-      <c r="N56" s="32"/>
-      <c r="O56" s="32"/>
-      <c r="P56" s="32"/>
-      <c r="Q56" s="32"/>
-      <c r="R56" s="32"/>
-      <c r="S56" s="32"/>
-      <c r="T56" s="32"/>
-      <c r="U56" s="32"/>
-      <c r="V56" s="32"/>
-      <c r="W56" s="32"/>
-      <c r="X56" s="32"/>
-      <c r="Y56" s="32"/>
-      <c r="Z56" s="32"/>
-      <c r="AA56" s="30"/>
-      <c r="AB56" s="30"/>
-    </row>
-    <row r="57" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="B57" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="C57" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="D57" s="24"/>
-      <c r="E57" s="33"/>
-      <c r="F57" s="34"/>
-      <c r="G57" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="H57" s="32"/>
-      <c r="I57" s="32"/>
-      <c r="J57" s="32"/>
-      <c r="K57" s="27"/>
-      <c r="L57" s="32"/>
-      <c r="M57" s="32"/>
-      <c r="N57" s="32"/>
-      <c r="O57" s="32"/>
-      <c r="P57" s="32"/>
-      <c r="Q57" s="32"/>
-      <c r="R57" s="32"/>
-      <c r="S57" s="32"/>
-      <c r="T57" s="32"/>
-      <c r="U57" s="32"/>
-      <c r="V57" s="32"/>
-      <c r="W57" s="32"/>
-      <c r="X57" s="32"/>
-      <c r="Y57" s="32"/>
-      <c r="Z57" s="32"/>
-      <c r="AA57" s="30"/>
-      <c r="AB57" s="30"/>
-    </row>
-    <row r="58" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="B58" s="33" t="s">
-        <v>124</v>
-      </c>
-      <c r="C58" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="D58" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="E58" s="33"/>
-      <c r="F58" s="34"/>
-      <c r="G58" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="H58" s="32"/>
-      <c r="I58" s="32"/>
-      <c r="J58" s="32"/>
-      <c r="K58" s="27"/>
-      <c r="L58" s="32"/>
-      <c r="M58" s="32"/>
-      <c r="N58" s="32"/>
-      <c r="O58" s="32"/>
-      <c r="P58" s="32"/>
-      <c r="Q58" s="32"/>
-      <c r="R58" s="32"/>
-      <c r="S58" s="32"/>
-      <c r="T58" s="32"/>
-      <c r="U58" s="32"/>
-      <c r="V58" s="32"/>
-      <c r="W58" s="32"/>
-      <c r="X58" s="32"/>
-      <c r="Y58" s="32"/>
-      <c r="Z58" s="32"/>
-      <c r="AA58" s="30"/>
-      <c r="AB58" s="30"/>
-    </row>
-    <row r="59" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="B59" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="C59" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="D59" s="24"/>
-      <c r="E59" s="33"/>
-      <c r="F59" s="34"/>
-      <c r="G59" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="H59" s="32"/>
-      <c r="I59" s="32"/>
-      <c r="J59" s="32"/>
-      <c r="K59" s="27"/>
-      <c r="L59" s="32"/>
-      <c r="M59" s="32"/>
-      <c r="N59" s="32"/>
-      <c r="O59" s="32"/>
-      <c r="P59" s="32"/>
-      <c r="Q59" s="32"/>
-      <c r="R59" s="32"/>
-      <c r="S59" s="32"/>
-      <c r="T59" s="32"/>
-      <c r="U59" s="32"/>
-      <c r="V59" s="32"/>
-      <c r="W59" s="32"/>
-      <c r="X59" s="32"/>
-      <c r="Y59" s="32"/>
-      <c r="Z59" s="32"/>
-      <c r="AA59" s="30"/>
-      <c r="AB59" s="30"/>
-    </row>
-    <row r="60" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="B60" s="33" t="s">
-        <v>130</v>
-      </c>
-      <c r="C60" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="D60" s="24"/>
-      <c r="E60" s="33"/>
-      <c r="F60" s="34"/>
-      <c r="G60" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="H60" s="32"/>
-      <c r="I60" s="32"/>
-      <c r="J60" s="32"/>
-      <c r="K60" s="27"/>
-      <c r="L60" s="32"/>
-      <c r="M60" s="32"/>
-      <c r="N60" s="32"/>
-      <c r="O60" s="32"/>
-      <c r="P60" s="32"/>
-      <c r="Q60" s="32"/>
-      <c r="R60" s="32"/>
-      <c r="S60" s="32"/>
-      <c r="T60" s="32"/>
-      <c r="U60" s="32"/>
-      <c r="V60" s="32"/>
-      <c r="W60" s="32"/>
-      <c r="X60" s="32"/>
-      <c r="Y60" s="32"/>
-      <c r="Z60" s="32"/>
-      <c r="AA60" s="30"/>
-      <c r="AB60" s="30"/>
-    </row>
-    <row r="61" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="B61" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="C61" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="D61" s="22"/>
-      <c r="E61" s="22"/>
-      <c r="F61" s="25"/>
-      <c r="G61" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="H61" s="32"/>
-      <c r="I61" s="32"/>
-      <c r="J61" s="32"/>
-      <c r="K61" s="27"/>
-      <c r="L61" s="32"/>
-      <c r="M61" s="32"/>
-      <c r="N61" s="32"/>
-      <c r="O61" s="32"/>
-      <c r="P61" s="32"/>
-      <c r="Q61" s="32"/>
-      <c r="R61" s="32"/>
-      <c r="S61" s="32"/>
-      <c r="T61" s="32"/>
-      <c r="U61" s="32"/>
-      <c r="V61" s="32"/>
-      <c r="W61" s="32"/>
-      <c r="X61" s="32"/>
-      <c r="Y61" s="32"/>
-      <c r="Z61" s="32"/>
-      <c r="AA61" s="30"/>
-      <c r="AB61" s="30"/>
-    </row>
-    <row r="62" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="B62" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="C62" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="D62" s="22"/>
-      <c r="E62" s="22"/>
-      <c r="F62" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="G62" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="H62" s="32"/>
-      <c r="I62" s="32"/>
-      <c r="J62" s="32"/>
-      <c r="K62" s="27"/>
-      <c r="L62" s="32"/>
-      <c r="M62" s="32"/>
-      <c r="N62" s="32"/>
-      <c r="O62" s="32"/>
-      <c r="P62" s="32"/>
-      <c r="Q62" s="32"/>
-      <c r="R62" s="32"/>
-      <c r="S62" s="32"/>
-      <c r="T62" s="32"/>
-      <c r="U62" s="32"/>
-      <c r="V62" s="32"/>
-      <c r="W62" s="32"/>
-      <c r="X62" s="32"/>
-      <c r="Y62" s="32"/>
-      <c r="Z62" s="32"/>
-      <c r="AA62" s="30"/>
-      <c r="AB62" s="30"/>
-    </row>
-    <row r="63" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="B63" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="C63" s="23" t="s">
-        <v>139</v>
-      </c>
-      <c r="D63" s="22"/>
-      <c r="E63" s="22"/>
-      <c r="F63" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="G63" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="H63" s="32"/>
-      <c r="I63" s="32"/>
-      <c r="J63" s="32"/>
-      <c r="K63" s="27"/>
-      <c r="L63" s="32"/>
-      <c r="M63" s="32"/>
-      <c r="N63" s="32"/>
-      <c r="O63" s="32"/>
-      <c r="P63" s="32"/>
-      <c r="Q63" s="32"/>
-      <c r="R63" s="32"/>
-      <c r="S63" s="32"/>
-      <c r="T63" s="32"/>
-      <c r="U63" s="32"/>
-      <c r="V63" s="32"/>
-      <c r="W63" s="32"/>
-      <c r="X63" s="32"/>
-      <c r="Y63" s="32"/>
-      <c r="Z63" s="32"/>
-      <c r="AA63" s="30"/>
-      <c r="AB63" s="30"/>
-    </row>
-    <row r="64" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="B64" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="C64" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="D64" s="22"/>
-      <c r="E64" s="22"/>
-      <c r="F64" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="G64" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="H64" s="32"/>
-      <c r="I64" s="32"/>
-      <c r="J64" s="32"/>
-      <c r="K64" s="27"/>
-      <c r="L64" s="32"/>
-      <c r="M64" s="32"/>
-      <c r="N64" s="32"/>
-      <c r="O64" s="32"/>
-      <c r="P64" s="32"/>
-      <c r="Q64" s="32"/>
-      <c r="R64" s="32"/>
-      <c r="S64" s="32"/>
-      <c r="T64" s="32"/>
-      <c r="U64" s="32"/>
-      <c r="V64" s="32"/>
-      <c r="W64" s="32"/>
-      <c r="X64" s="32"/>
-      <c r="Y64" s="32"/>
-      <c r="Z64" s="32"/>
-      <c r="AA64" s="30"/>
-      <c r="AB64" s="30"/>
-    </row>
-    <row r="65" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="B65" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="C65" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="D65" s="22"/>
-      <c r="E65" s="22"/>
-      <c r="F65" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="G65" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="H65" s="32"/>
-      <c r="I65" s="32"/>
-      <c r="J65" s="32"/>
-      <c r="K65" s="27"/>
-      <c r="L65" s="32"/>
-      <c r="M65" s="32"/>
-      <c r="N65" s="32"/>
-      <c r="O65" s="32"/>
-      <c r="P65" s="32"/>
-      <c r="Q65" s="32"/>
-      <c r="R65" s="32"/>
-      <c r="S65" s="32"/>
-      <c r="T65" s="32"/>
-      <c r="U65" s="32"/>
-      <c r="V65" s="32"/>
-      <c r="W65" s="32"/>
-      <c r="X65" s="32"/>
-      <c r="Y65" s="32"/>
-      <c r="Z65" s="32"/>
-      <c r="AA65" s="30"/>
-      <c r="AB65" s="30"/>
-    </row>
-    <row r="66" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="B66" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="C66" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="D66" s="22"/>
-      <c r="E66" s="22"/>
-      <c r="F66" s="25"/>
-      <c r="G66" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="H66" s="32"/>
-      <c r="I66" s="32"/>
-      <c r="J66" s="32"/>
-      <c r="K66" s="27"/>
-      <c r="L66" s="32"/>
-      <c r="M66" s="32"/>
-      <c r="N66" s="32"/>
-      <c r="O66" s="32"/>
-      <c r="P66" s="32"/>
-      <c r="Q66" s="32"/>
-      <c r="R66" s="32"/>
-      <c r="S66" s="32"/>
-      <c r="T66" s="32"/>
-      <c r="U66" s="32"/>
-      <c r="V66" s="32"/>
-      <c r="W66" s="32"/>
-      <c r="X66" s="32"/>
-      <c r="Y66" s="32"/>
-      <c r="Z66" s="32"/>
-      <c r="AA66" s="30"/>
-      <c r="AB66" s="30"/>
-    </row>
-    <row r="67" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="B67" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="C67" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="D67" s="22"/>
-      <c r="E67" s="22"/>
-      <c r="F67" s="25"/>
-      <c r="G67" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="H67" s="32"/>
-      <c r="I67" s="32"/>
-      <c r="J67" s="32"/>
-      <c r="K67" s="27"/>
-      <c r="L67" s="32"/>
-      <c r="M67" s="32"/>
-      <c r="N67" s="32"/>
-      <c r="O67" s="32"/>
-      <c r="P67" s="32"/>
-      <c r="Q67" s="32"/>
-      <c r="R67" s="32"/>
-      <c r="S67" s="32"/>
-      <c r="T67" s="32"/>
-      <c r="U67" s="32"/>
-      <c r="V67" s="32"/>
-      <c r="W67" s="32"/>
-      <c r="X67" s="32"/>
-      <c r="Y67" s="32"/>
-      <c r="Z67" s="32"/>
-      <c r="AA67" s="30"/>
-      <c r="AB67" s="30"/>
-    </row>
-    <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="H68" s="29"/>
-      <c r="I68" s="29"/>
-      <c r="J68" s="32"/>
-      <c r="K68" s="27"/>
-      <c r="L68" s="29"/>
-      <c r="M68" s="29"/>
-      <c r="N68" s="29"/>
-      <c r="O68" s="29"/>
-      <c r="P68" s="29"/>
-      <c r="Q68" s="29"/>
-      <c r="R68" s="29"/>
-      <c r="S68" s="29"/>
-      <c r="T68" s="29"/>
-      <c r="U68" s="29"/>
-      <c r="V68" s="29"/>
-      <c r="W68" s="29"/>
-      <c r="X68" s="29"/>
-      <c r="Y68" s="29"/>
-      <c r="Z68" s="29"/>
-      <c r="AA68" s="30"/>
-      <c r="AB68" s="30"/>
+      <c r="H75" s="31"/>
+      <c r="I75" s="31"/>
+      <c r="J75" s="34"/>
+      <c r="K75" s="29"/>
+      <c r="L75" s="31"/>
+      <c r="M75" s="31"/>
+      <c r="N75" s="31"/>
+      <c r="O75" s="31"/>
+      <c r="P75" s="31"/>
+      <c r="Q75" s="31"/>
+      <c r="R75" s="31"/>
+      <c r="S75" s="31"/>
+      <c r="T75" s="31"/>
+      <c r="U75" s="31"/>
+      <c r="V75" s="31"/>
+      <c r="W75" s="31"/>
+      <c r="X75" s="31"/>
+      <c r="Y75" s="31"/>
+      <c r="Z75" s="31"/>
+      <c r="AA75" s="32"/>
+      <c r="AB75" s="32"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E47:E52 E54" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E47:E59 E61" type="list">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3904,178 +4330,208 @@
   <dimension ref="A1:V1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.61328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="28.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="2" style="35" width="45.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="37" width="28.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="2" style="37" width="45.84"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="36" t="s">
-        <v>151</v>
-      </c>
-      <c r="B1" s="36" t="s">
+      <c r="A1" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="F1" s="40" t="s">
+      <c r="D1" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="41" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1" s="42" t="s">
-        <v>155</v>
-      </c>
-      <c r="I1" s="43" t="s">
-        <v>156</v>
-      </c>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
+      <c r="G1" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="I1" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="46"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="46" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="47" t="s">
+        <v>179</v>
+      </c>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
+      <c r="U2" s="48"/>
+      <c r="V2" s="48"/>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="46" t="s">
+        <v>178</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="48"/>
+      <c r="T3" s="48"/>
+      <c r="U3" s="48"/>
+      <c r="V3" s="48"/>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="46"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="48"/>
+      <c r="S4" s="48"/>
+      <c r="T4" s="48"/>
+      <c r="U4" s="48"/>
+      <c r="V4" s="48"/>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="44" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="45" t="s">
-        <v>158</v>
-      </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="46"/>
-      <c r="V2" s="46"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="44" t="s">
-        <v>157</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="C3" s="45" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="C6" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="46"/>
-      <c r="S3" s="46"/>
-      <c r="T3" s="46"/>
-      <c r="U3" s="46"/>
-      <c r="V3" s="46"/>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="44"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="46"/>
-      <c r="N4" s="46"/>
-      <c r="O4" s="46"/>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="46"/>
-      <c r="R4" s="46"/>
-      <c r="S4" s="46"/>
-      <c r="T4" s="46"/>
-      <c r="U4" s="46"/>
-      <c r="V4" s="46"/>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="B5" s="35" t="s">
-        <v>161</v>
-      </c>
-      <c r="C5" s="35" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="B6" s="35" t="s">
-        <v>162</v>
-      </c>
-      <c r="C6" s="35" t="s">
-        <v>139</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="B7" s="35" t="s">
+      <c r="A7" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="C7" s="35" t="s">
-        <v>142</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>190</v>
+      </c>
+    </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4148,94 +4604,94 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="36" t="s">
-        <v>164</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>165</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>166</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>167</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>168</v>
-      </c>
-      <c r="F1" s="36" t="s">
-        <v>169</v>
-      </c>
-      <c r="G1" s="47" t="s">
-        <v>170</v>
-      </c>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="36"/>
-      <c r="V1" s="36"/>
-      <c r="W1" s="36"/>
-      <c r="X1" s="36"/>
-      <c r="Y1" s="36"/>
-      <c r="Z1" s="36"/>
+      <c r="A1" s="38" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>195</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>196</v>
+      </c>
+      <c r="G1" s="49" t="s">
+        <v>197</v>
+      </c>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" s="49" t="n">
+      <c r="A2" s="50" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="51" t="n">
         <f aca="true">NOW()</f>
-        <v>45138.6238921957</v>
-      </c>
-      <c r="D2" s="50" t="s">
-        <v>171</v>
-      </c>
-      <c r="E2" s="50" t="s">
-        <v>172</v>
-      </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="51" t="s">
-        <v>173</v>
-      </c>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="44"/>
-      <c r="S2" s="44"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="44"/>
-      <c r="V2" s="44"/>
-      <c r="W2" s="44"/>
-      <c r="X2" s="44"/>
-      <c r="Y2" s="44"/>
-      <c r="Z2" s="44"/>
+        <v>45218.4060623423</v>
+      </c>
+      <c r="D2" s="52" t="s">
+        <v>198</v>
+      </c>
+      <c r="E2" s="52" t="s">
+        <v>199</v>
+      </c>
+      <c r="F2" s="46"/>
+      <c r="G2" s="53" t="s">
+        <v>200</v>
+      </c>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="46"/>
+      <c r="T2" s="46"/>
+      <c r="U2" s="46"/>
+      <c r="V2" s="46"/>
+      <c r="W2" s="46"/>
+      <c r="X2" s="46"/>
+      <c r="Y2" s="46"/>
+      <c r="Z2" s="46"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
updated forms and condition cards
</commit_message>
<xml_diff>
--- a/POSHIT/Example CHT application/malaria-usecase-cht/forms/app/children_under_5_follow_up.xlsx
+++ b/POSHIT/Example CHT application/malaria-usecase-cht/forms/app/children_under_5_follow_up.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="202">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -702,6 +702,9 @@
   </si>
   <si>
     <t xml:space="preserve">default_language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U5 follow up</t>
   </si>
   <si>
     <t xml:space="preserve">pages</t>
@@ -1260,11 +1263,11 @@
   </sheetPr>
   <dimension ref="A1:AJ75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C67" activeCellId="0" sqref="C67"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C53" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F75" activeCellId="0" sqref="F75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.55"/>
@@ -4207,7 +4210,9 @@
       </c>
       <c r="D73" s="24"/>
       <c r="E73" s="24"/>
-      <c r="F73" s="27"/>
+      <c r="F73" s="27" t="s">
+        <v>161</v>
+      </c>
       <c r="G73" s="24" t="s">
         <v>155</v>
       </c>
@@ -4245,7 +4250,9 @@
       </c>
       <c r="D74" s="24"/>
       <c r="E74" s="24"/>
-      <c r="F74" s="27"/>
+      <c r="F74" s="27" t="s">
+        <v>161</v>
+      </c>
       <c r="G74" s="24" t="s">
         <v>144</v>
       </c>
@@ -4333,7 +4340,7 @@
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="37" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="2" style="37" width="45.84"/>
@@ -4601,10 +4608,10 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.83"/>
@@ -4654,24 +4661,24 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="50" t="s">
-        <v>98</v>
+        <v>198</v>
       </c>
       <c r="B2" s="50" t="s">
         <v>97</v>
       </c>
       <c r="C2" s="51" t="n">
         <f aca="true">NOW()</f>
-        <v>45218.4060623423</v>
+        <v>45231.5712246041</v>
       </c>
       <c r="D2" s="52" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E2" s="52" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F2" s="46"/>
       <c r="G2" s="53" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H2" s="46"/>
       <c r="I2" s="46"/>

</xml_diff>